<commit_message>
Update Lab 4 report
</commit_message>
<xml_diff>
--- a/lab4/pipeline.xlsx
+++ b/lab4/pipeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>Cycle</t>
   </si>
@@ -264,16 +264,7 @@
     <t>We will ignore the the fact that sides A and B are both used at the same time and just consider the iterations.</t>
   </si>
   <si>
-    <t>The loading operation takes 2 pipeline stages.</t>
-  </si>
-  <si>
-    <t>The multiply operations takes 3 pipleine stages, but the results can be used in the same iteration</t>
-  </si>
-  <si>
     <t>Each iteration of the loop will move the pipeline stages forward by one</t>
-  </si>
-  <si>
-    <t>The addition operation takes 2 pipeline stages.</t>
   </si>
   <si>
     <r>
@@ -296,6 +287,18 @@
       </rPr>
       <t>refers to spurious operations that cannot be prevent</t>
     </r>
+  </si>
+  <si>
+    <t>The loading operation (L) takes 2 pipeline stages.</t>
+  </si>
+  <si>
+    <t>The multiply operation (x)  takes 3 pipleine stages, but the results can be used in the same iteration</t>
+  </si>
+  <si>
+    <t>The addition operation (+)  takes 2 pipeline stages.</t>
+  </si>
+  <si>
+    <t>The number indicates the ith iteration of the MAC operation</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1303,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1322,7 +1325,7 @@
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1348,7 +1351,7 @@
         <v>57</v>
       </c>
       <c r="I21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1374,7 +1377,7 @@
         <v>58</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1388,7 +1391,7 @@
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="I23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1412,6 +1415,9 @@
       </c>
       <c r="G24" s="19" t="s">
         <v>69</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>